<commit_message>
Completion of all tasks
</commit_message>
<xml_diff>
--- a/FirstTask.xlsx
+++ b/FirstTask.xlsx
@@ -4,14 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="Автобусы" sheetId="1" r:id="rId1"/>
-    <sheet name="Маршруты" sheetId="2" r:id="rId2"/>
-    <sheet name="Водители" sheetId="3" r:id="rId3"/>
-    <sheet name="Контролеры" sheetId="4" r:id="rId4"/>
-    <sheet name="Расписание" sheetId="5" r:id="rId5"/>
+    <sheet name="Расписание" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -137,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -161,17 +157,38 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,14 +199,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -497,334 +519,29 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>445</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
     <col min="1" max="1" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -943,6 +660,202 @@
       </c>
       <c r="E8" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>2</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>6</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>1</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>2</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>3</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>4</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>5</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>6</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>